<commit_message>
feat: readme and categories
</commit_message>
<xml_diff>
--- a/z_test_by_category.xlsx
+++ b/z_test_by_category.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,335 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Категория</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Кол-во сотрудников</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Средняя разница</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Z-статистика</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>P-значение</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Вывод</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Мерч и сувениры КРОК</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>589</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-221.01</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-7.337</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>❌ Отрицательный рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Без категории</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>671</v>
+      </c>
+      <c r="C3" t="n">
+        <v>296.79</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✅ Рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>В стиле КРОК</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>372</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-59.81</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1.845</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>❌ Нет роста</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Сервис</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>232</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-130.75</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2.761</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>❌ Отрицательный рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Лучше вместе</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>256</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-54.16</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1.091</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>❌ Нет роста</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Поймай баланс</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>359</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-238.54</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-7.766</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>❌ Отрицательный рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>КРОК FEST TOUR</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>45</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-603.78</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-3.281</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>❌ Отрицательный рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Развивай себя</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-39.9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.697</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>❌ Нет роста</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Прокачай эффективность</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>180</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-105.28</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-2.008</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>❌ Отрицательный рост</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Смена деятельности</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>99</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-12.37</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>❌ Нет роста</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Своими руками</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>45</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-11.89</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.075</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>❌ Нет роста</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Новогодние атрибуты</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>41</v>
+      </c>
+      <c r="C13" t="n">
+        <v>281.71</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>✅ Рост</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>